<commit_message>
fixing bugs and testing things
</commit_message>
<xml_diff>
--- a/Implementation/Data/Optimal-Betas.xlsx
+++ b/Implementation/Data/Optimal-Betas.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Betas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Betas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-899.9999999999994</v>
+        <v>-15155.30149999998</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.03000000000000264</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.03300000000000036</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>3</v>
+        <v>1.899999999999993</v>
       </c>
     </row>
     <row r="4">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>2</v>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.03630000000000022</v>
       </c>
       <c r="M4" t="n">
         <v>1</v>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="5">
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>6.661338147750939e-16</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>3</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.03993000000000002</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="6">
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.04392300000000127</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="7">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>0.04831530000000017</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="8">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>0.0531468300000002</v>
       </c>
       <c r="M8" t="n">
         <v>1</v>
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="9">
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.05846151300000058</v>
       </c>
       <c r="M9" t="n">
         <v>1</v>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>3</v>
+        <v>1.899999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.06430766429999979</v>
       </c>
       <c r="M10" t="n">
         <v>1</v>
@@ -984,7 +984,7 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>3</v>
+        <v>1.899999999999998</v>
       </c>
     </row>
     <row r="11">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>1.923579476910001</v>
       </c>
       <c r="M11" t="n">
         <v>1</v>
@@ -1043,7 +1043,7 @@
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="12">
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>4.519679884700995</v>
       </c>
       <c r="M12" t="n">
         <v>1</v>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>5.593742460100003</v>
+        <v>4.4937424601</v>
       </c>
     </row>
     <row r="13">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>-8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>-8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>-8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="Q28" t="n">
-        <v>-4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="Q29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="Q38" t="n">
-        <v>3.552713678800501e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="Q39" t="n">
-        <v>4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="Q49" t="n">
-        <v>-8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="Q50" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1899,7 +1899,7 @@
         </is>
       </c>
       <c r="Q51" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="Q52" t="n">
-        <v>1.77635683940025e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="Q60" t="n">
-        <v>4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2109,7 +2109,7 @@
         </is>
       </c>
       <c r="Q61" t="n">
-        <v>4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="Q62" t="n">
-        <v>8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="Q65" t="n">
-        <v>2.220446049250313e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2235,7 +2235,7 @@
         </is>
       </c>
       <c r="Q67" t="n">
-        <v>2.593742460100003</v>
+        <v>2.593742460100002</v>
       </c>
     </row>
     <row r="68">
@@ -2298,7 +2298,7 @@
         </is>
       </c>
       <c r="Q70" t="n">
-        <v>8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2319,7 +2319,7 @@
         </is>
       </c>
       <c r="Q71" t="n">
-        <v>2.220446049250313e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="Q72" t="n">
-        <v>8.881784197001252e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="Q74" t="n">
-        <v>4.440892098500626e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="Q78" t="n">
-        <v>0</v>
+        <v>2.593742460100003</v>
       </c>
     </row>
     <row r="79">
@@ -2529,7 +2529,7 @@
         </is>
       </c>
       <c r="Q81" t="n">
-        <v>1.110223024625157e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="Q89" t="n">
-        <v>0</v>
+        <v>2.593742460100003</v>
       </c>
     </row>
     <row r="90">
@@ -2739,7 +2739,7 @@
         </is>
       </c>
       <c r="Q91" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2928,7 +2928,7 @@
         </is>
       </c>
       <c r="Q100" t="n">
-        <v>0</v>
+        <v>2.593742460100003</v>
       </c>
     </row>
     <row r="101">

</xml_diff>